<commit_message>
Bug fixing on creating SP list/library
</commit_message>
<xml_diff>
--- a/SharePoint/empty.xlsx
+++ b/SharePoint/empty.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Types" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Metadata!$B$3:$N$53</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Metadata!$B$3:$N$102</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Types!$A$1:$C$35</definedName>
     <definedName function="false" hidden="false" name="Types" vbProcedure="false">Types!$A$1:$C$35</definedName>
     <definedName function="false" hidden="false" name="TypesFR" vbProcedure="false">Types!$A$2:$A$13</definedName>
@@ -215,8 +215,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -259,7 +260,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF0563C1"/>
+      <color rgb="FF3465A4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -438,7 +439,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -455,10 +456,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -467,10 +476,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,36 +484,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -621,11 +614,29 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -669,7 +680,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -693,10 +704,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1048576"/>
+  <dimension ref="A1:Q103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -706,975 +721,1123 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="29.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="7" style="1" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="6.01"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="11.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="7" style="4" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="18" style="1" width="11.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" s="6" customFormat="true" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" s="7" customFormat="true" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="8" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" s="6" customFormat="true" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="str">
+      <c r="G3" s="10"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C4,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="str">
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+    </row>
+    <row r="5" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C5,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="str">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+    </row>
+    <row r="6" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C6,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="str">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+    </row>
+    <row r="7" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C7,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="str">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+    </row>
+    <row r="8" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C8,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="str">
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+    </row>
+    <row r="9" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C9,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="str">
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+    </row>
+    <row r="10" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C10,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="str">
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+    </row>
+    <row r="11" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C11,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="str">
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+    </row>
+    <row r="12" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C12,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="str">
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+    </row>
+    <row r="13" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C13,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="str">
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+    </row>
+    <row r="14" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C14,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="str">
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+    </row>
+    <row r="15" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C15,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="str">
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+    </row>
+    <row r="16" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C16,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="str">
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+    </row>
+    <row r="17" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C17,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="str">
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+    </row>
+    <row r="18" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C18,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="str">
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+    </row>
+    <row r="19" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C19,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="str">
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+    </row>
+    <row r="20" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C20,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="str">
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+    </row>
+    <row r="21" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C21,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="str">
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+    </row>
+    <row r="22" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C22,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="str">
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+    </row>
+    <row r="23" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C23,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="str">
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+    </row>
+    <row r="24" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C24,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="str">
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+    </row>
+    <row r="25" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C25,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="str">
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+    </row>
+    <row r="26" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C26,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="str">
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+    </row>
+    <row r="27" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C27,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="str">
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+    </row>
+    <row r="28" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C28,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="str">
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+    </row>
+    <row r="29" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C29,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="str">
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+    </row>
+    <row r="30" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C30,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-    </row>
-    <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="str">
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+    </row>
+    <row r="31" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C31,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="str">
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+    </row>
+    <row r="32" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C32,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="str">
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+    </row>
+    <row r="33" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C33,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="str">
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+    </row>
+    <row r="34" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C34,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="str">
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+    </row>
+    <row r="35" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C35,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="str">
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+    </row>
+    <row r="36" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C36,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="str">
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+    </row>
+    <row r="37" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C37,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="str">
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+    </row>
+    <row r="38" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C38,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="str">
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+    </row>
+    <row r="39" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C39,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="str">
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+    </row>
+    <row r="40" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C40,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="str">
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+    </row>
+    <row r="41" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C41,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="str">
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+    </row>
+    <row r="42" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C42,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="str">
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+    </row>
+    <row r="43" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C43,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="str">
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+    </row>
+    <row r="44" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C44,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="str">
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+    </row>
+    <row r="45" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C45,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="str">
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+    </row>
+    <row r="46" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C46,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="str">
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+    </row>
+    <row r="47" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C47,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="str">
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+    </row>
+    <row r="48" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C48,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="str">
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+    </row>
+    <row r="49" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C49,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="str">
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+    </row>
+    <row r="50" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C50,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="str">
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+    </row>
+    <row r="51" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="11" t="str">
         <f aca="false">IFERROR(VLOOKUP(C51,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
@@ -1683,62 +1846,1151 @@
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
-    </row>
-    <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="18" t="s">
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
+    </row>
+    <row r="52" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C52,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+    </row>
+    <row r="53" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C53,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+    </row>
+    <row r="54" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C54,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+    </row>
+    <row r="55" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C55,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+    </row>
+    <row r="56" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C56,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="15"/>
+      <c r="O56" s="15"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="15"/>
+    </row>
+    <row r="57" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C57,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="15"/>
+    </row>
+    <row r="58" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C58,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
+      <c r="Q58" s="15"/>
+    </row>
+    <row r="59" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C59,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15"/>
+      <c r="Q59" s="15"/>
+    </row>
+    <row r="60" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C60,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="15"/>
+    </row>
+    <row r="61" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C61,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+    </row>
+    <row r="62" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C62,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="15"/>
+    </row>
+    <row r="63" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C63,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
+    </row>
+    <row r="64" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C64,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+    </row>
+    <row r="65" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C65,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="15"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+    </row>
+    <row r="66" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C66,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
+    </row>
+    <row r="67" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C67,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="15"/>
+      <c r="P67" s="15"/>
+      <c r="Q67" s="15"/>
+    </row>
+    <row r="68" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C68,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+    </row>
+    <row r="69" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C69,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="15"/>
+    </row>
+    <row r="70" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C70,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+    </row>
+    <row r="71" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C71,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+    </row>
+    <row r="72" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C72,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+    </row>
+    <row r="73" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C73,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+    </row>
+    <row r="74" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C74,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+    </row>
+    <row r="75" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C75,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+    </row>
+    <row r="76" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C76,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+    </row>
+    <row r="77" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C77,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+    </row>
+    <row r="78" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C78,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+    </row>
+    <row r="79" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C79,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15"/>
+      <c r="Q79" s="15"/>
+    </row>
+    <row r="80" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C80,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
+      <c r="P80" s="15"/>
+      <c r="Q80" s="15"/>
+    </row>
+    <row r="81" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C81,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
+      <c r="P81" s="15"/>
+      <c r="Q81" s="15"/>
+    </row>
+    <row r="82" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C82,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B82" s="13"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
+      <c r="P82" s="15"/>
+      <c r="Q82" s="15"/>
+    </row>
+    <row r="83" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C83,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15"/>
+      <c r="P83" s="15"/>
+      <c r="Q83" s="15"/>
+    </row>
+    <row r="84" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C84,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="15"/>
+      <c r="M84" s="15"/>
+      <c r="N84" s="15"/>
+      <c r="O84" s="15"/>
+      <c r="P84" s="15"/>
+      <c r="Q84" s="15"/>
+    </row>
+    <row r="85" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C85,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+    </row>
+    <row r="86" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C86,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B86" s="13"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15"/>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+    </row>
+    <row r="87" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C87,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="15"/>
+      <c r="M87" s="15"/>
+      <c r="N87" s="15"/>
+      <c r="O87" s="15"/>
+      <c r="P87" s="15"/>
+      <c r="Q87" s="15"/>
+    </row>
+    <row r="88" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C88,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="15"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="15"/>
+      <c r="O88" s="15"/>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+    </row>
+    <row r="89" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C89,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B89" s="13"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="15"/>
+      <c r="M89" s="15"/>
+      <c r="N89" s="15"/>
+      <c r="O89" s="15"/>
+      <c r="P89" s="15"/>
+      <c r="Q89" s="15"/>
+    </row>
+    <row r="90" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C90,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="15"/>
+      <c r="H90" s="15"/>
+      <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="15"/>
+      <c r="L90" s="15"/>
+      <c r="M90" s="15"/>
+      <c r="N90" s="15"/>
+      <c r="O90" s="15"/>
+      <c r="P90" s="15"/>
+      <c r="Q90" s="15"/>
+    </row>
+    <row r="91" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C91,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="15"/>
+      <c r="M91" s="15"/>
+      <c r="N91" s="15"/>
+      <c r="O91" s="15"/>
+      <c r="P91" s="15"/>
+      <c r="Q91" s="15"/>
+    </row>
+    <row r="92" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C92,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="15"/>
+      <c r="N92" s="15"/>
+      <c r="O92" s="15"/>
+      <c r="P92" s="15"/>
+      <c r="Q92" s="15"/>
+    </row>
+    <row r="93" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C93,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="15"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="15"/>
+      <c r="M93" s="15"/>
+      <c r="N93" s="15"/>
+      <c r="O93" s="15"/>
+      <c r="P93" s="15"/>
+      <c r="Q93" s="15"/>
+    </row>
+    <row r="94" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C94,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
+      <c r="L94" s="15"/>
+      <c r="M94" s="15"/>
+      <c r="N94" s="15"/>
+      <c r="O94" s="15"/>
+      <c r="P94" s="15"/>
+      <c r="Q94" s="15"/>
+    </row>
+    <row r="95" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C95,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B95" s="13"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="15"/>
+      <c r="M95" s="15"/>
+      <c r="N95" s="15"/>
+      <c r="O95" s="15"/>
+      <c r="P95" s="15"/>
+      <c r="Q95" s="15"/>
+    </row>
+    <row r="96" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C96,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B96" s="13"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="15"/>
+      <c r="L96" s="15"/>
+      <c r="M96" s="15"/>
+      <c r="N96" s="15"/>
+      <c r="O96" s="15"/>
+      <c r="P96" s="15"/>
+      <c r="Q96" s="15"/>
+    </row>
+    <row r="97" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C97,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
+      <c r="J97" s="15"/>
+      <c r="K97" s="15"/>
+      <c r="L97" s="15"/>
+      <c r="M97" s="15"/>
+      <c r="N97" s="15"/>
+      <c r="O97" s="15"/>
+      <c r="P97" s="15"/>
+      <c r="Q97" s="15"/>
+    </row>
+    <row r="98" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C98,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="15"/>
+      <c r="N98" s="15"/>
+      <c r="O98" s="15"/>
+      <c r="P98" s="15"/>
+      <c r="Q98" s="15"/>
+    </row>
+    <row r="99" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C99,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="15"/>
+      <c r="L99" s="15"/>
+      <c r="M99" s="15"/>
+      <c r="N99" s="15"/>
+      <c r="O99" s="15"/>
+      <c r="P99" s="15"/>
+      <c r="Q99" s="15"/>
+    </row>
+    <row r="100" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="11" t="str">
+        <f aca="false">IFERROR(VLOOKUP(C100,Types,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
+      <c r="I100" s="15"/>
+      <c r="J100" s="15"/>
+      <c r="K100" s="15"/>
+      <c r="L100" s="15"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="15"/>
+      <c r="O100" s="15"/>
+      <c r="P100" s="15"/>
+      <c r="Q100" s="15"/>
+    </row>
+    <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B101" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
-      <c r="N52" s="18"/>
-    </row>
-    <row r="53" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="19" t="s">
+      <c r="C101" s="16"/>
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="16"/>
+      <c r="H101" s="16"/>
+      <c r="I101" s="16"/>
+      <c r="J101" s="16"/>
+      <c r="K101" s="16"/>
+      <c r="L101" s="16"/>
+      <c r="M101" s="16"/>
+      <c r="N101" s="16"/>
+      <c r="O101" s="16"/>
+      <c r="P101" s="16"/>
+      <c r="Q101" s="16"/>
+    </row>
+    <row r="102" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B102" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="20" t="s">
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="17"/>
+      <c r="J102" s="17"/>
+      <c r="K102" s="17"/>
+      <c r="L102" s="17"/>
+      <c r="M102" s="17"/>
+      <c r="N102" s="17"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="17"/>
+      <c r="Q102" s="17"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="20"/>
-      <c r="M54" s="20"/>
-      <c r="N54" s="20"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="18"/>
+      <c r="M103" s="18"/>
+      <c r="N103" s="18"/>
+      <c r="O103" s="18"/>
+      <c r="P103" s="18"/>
+      <c r="Q103" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="B1:N1"/>
+  <mergeCells count="105">
+    <mergeCell ref="B1:Q1"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -1791,12 +3043,94 @@
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="E51:F51"/>
-    <mergeCell ref="B52:N52"/>
-    <mergeCell ref="B53:N53"/>
-    <mergeCell ref="B54:N54"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="B101:Q101"/>
+    <mergeCell ref="B102:Q102"/>
+    <mergeCell ref="B103:Q103"/>
   </mergeCells>
+  <conditionalFormatting sqref="G4:G100">
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H100">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I100">
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:J100">
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K100">
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L100">
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M100">
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N100">
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:O100">
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P100">
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4:Q100">
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C51" type="list">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C100" type="list">
       <formula1>TypesFR</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1822,387 +3156,387 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.42"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="23" customFormat="true" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="31"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="31"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="31"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="31"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="31"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="29"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="31"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="29"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="31"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="31"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="31"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="31"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="31"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="31"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="31"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="31"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="32"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="34"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="32"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="34"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="32"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="34"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="34"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="30"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="34"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="30"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="34"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="30"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="34"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="30"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="34"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="30"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="32"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="34"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="34"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="34"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="32"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="34"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="32"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="34"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="32"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="35"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="33"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="32"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="35"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="33"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="32"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="35"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="33"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="32"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="35"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="33"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="36"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="38"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="36"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="36"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="38"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="36"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="36"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="38"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="36"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="36"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="38"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="36"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="36"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="38"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="36"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="36"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="38"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="36"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="36"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="36"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="36"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="38"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="36"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="36"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="38"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="36"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="36"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="36"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="36"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="38"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="36"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="36"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="38"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="36"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="36"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="38"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="36"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="36"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="38"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="36"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="36"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="38"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="36"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="36"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="38"/>
+      <c r="A56" s="34"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="36"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="36"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="38"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="36"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="36"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="38"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="36"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="36"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="38"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="36"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="38"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="36"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="36"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="38"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="36"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="36"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
+      <c r="A62" s="34"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="36"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="36"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="38"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="36"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="36"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="38"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="36"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="36"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="38"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="36"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="36"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="38"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="36"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="36"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="38"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="36"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="36"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="38"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="36"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="36"/>
-      <c r="B69" s="37"/>
-      <c r="C69" s="38"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="36"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="36"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="38"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="36"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="39"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="41"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="38"/>
+      <c r="C71" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2240,20 +3574,20 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating CreateSiteColumnsFromXlsx script and new scripts
</commit_message>
<xml_diff>
--- a/SharePoint/empty.xlsx
+++ b/SharePoint/empty.xlsx
@@ -1261,9 +1261,9 @@
   <dimension ref="A1:AM283"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
       <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
@@ -14110,10 +14110,10 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.42"/>
   </cols>
   <sheetData>
@@ -14528,9 +14528,9 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
   </cols>
   <sheetData>

</xml_diff>